<commit_message>
Update Excel files for accelerators, angels, and targets; enhance sheet-utils.ts to improve string transformation and validation messaging for better user guidance.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/production/accelerators.xlsx
+++ b/src/lib/scripts/seed-data/production/accelerators.xlsx
@@ -1,22 +1,232 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A469332D-68CA-DE44-A65D-9A3B742134D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="20" yWindow="700" windowWidth="27040" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="accelerators template" sheetId="1" r:id="rId1"/>
-    <sheet name="ValidationData" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet sheetId="1" name="accelerators template" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="ValidationData" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- form
+- email
+- other</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- in-person
+- remote
+- hybrid</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- 3 months
+- 6 months
+- 12 months
+- ongoing
+- variable</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- 1-10
+- 11-20
+- 21-50
+- 51-100
+- 100+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- Pre-seed
+- Seed
+- Series A
+- Series B
+- Series C
+- Growth
+- All</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- B2B SaaS
+- Fintech
+- Healthtech
+- AI/ML
+- Deep tech
+- Climate tech
+- Consumer
+- E-commerce
+- Marketplace
+- Gaming
+- Web3
+- Developer tools
+- Cybersecurity
+- Logistics
+- AdTech
+- PropTech
+- InsurTech
+- Agriculture
+- Automotive
+- Biotechnology
+- Construction
+- Consulting
+- Consumer Goods
+- Education
+- Energy
+- Entertainment
+- Environmental Services
+- Fashion
+- Food &amp; Beverage
+- Government
+- Healthcare Services
+- Hospitality
+- Human Resources
+- Insurance
+- Legal
+- Manufacturing
+- Media
+- Non-profit
+- Pharmaceuticals
+- Real Estate
+- Retail
+- Telecommunications
+- Transportation
+- Utilities
+- Other</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- Global
+- North America
+- South America
+- LATAM
+- Europe
+- Western Europe
+- Eastern Europe
+- Continental Europe
+- Middle East
+- Africa
+- Asia
+- East Asia
+- South Asia
+- South East Asia
+- Oceania
+- EMEA
+- Emerging Markets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- 0%
+- 1-3%
+- 4-6%
+- 7-10%
+- 10%+
+- variable</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- 0-25K
+- 25K-50K
+- 50K-100K
+- 100K-250K
+- 250K-500K
+- 500K+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- &lt;1%
+- 1-5%
+- 6-10%
+- 11-20%
+- 20%+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- simple
+- standard
+- comprehensive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- pitch_deck
+- video
+- financial_projections
+- business_plan
+- traction_data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">Possible values:
+- FREE
+- PRO
+- MAX</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="137">
   <si>
     <t>name</t>
   </si>
@@ -432,42 +642,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -482,20 +675,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,46 +1016,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y1000"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="68" width="8.83203125" style="4"/>
-    <col min="69" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="25" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,187 +1099,1099 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AJ1" s="3"/>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
-      <c r="AS1" s="3"/>
-      <c r="AT1" s="3"/>
-      <c r="AU1" s="3"/>
-      <c r="AV1" s="3"/>
-      <c r="AW1" s="3"/>
-      <c r="AX1" s="3"/>
-      <c r="AY1" s="3"/>
-      <c r="AZ1" s="3"/>
-      <c r="BA1" s="3"/>
-      <c r="BB1" s="3"/>
-      <c r="BC1" s="3"/>
-      <c r="BD1" s="3"/>
-      <c r="BE1" s="3"/>
-      <c r="BF1" s="3"/>
-      <c r="BG1" s="3"/>
-      <c r="BH1" s="3"/>
-      <c r="BI1" s="3"/>
-      <c r="BJ1" s="3"/>
-      <c r="BK1" s="3"/>
-      <c r="BL1" s="3"/>
-      <c r="BM1" s="3"/>
-      <c r="BN1" s="3"/>
-      <c r="BO1" s="3"/>
-      <c r="BP1" s="3"/>
-    </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="E2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
+    </row>
+    <row r="2" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="227" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="228" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="229" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="238" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="241" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="243" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="257" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="258" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="259" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="260" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="261" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="262" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="263" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="264" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="265" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="271" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="275" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="276" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="277" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="278" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="279" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="301" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="302" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="303" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="304" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="305" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="306" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="307" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="308" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="309" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="310" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="311" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="312" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="313" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="314" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="315" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="316" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="317" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="318" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="319" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="320" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="321" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="322" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="323" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="324" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="325" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="326" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="327" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="328" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="329" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="330" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="331" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="332" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="333" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="334" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="335" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="336" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="337" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="338" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="339" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="340" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="341" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="342" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="343" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="344" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="345" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="346" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="347" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="348" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="349" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="350" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="351" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="352" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="353" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="354" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="355" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="356" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="357" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="358" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="359" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="360" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="361" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="362" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="363" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="364" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="365" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="366" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="367" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="368" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="369" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="370" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="371" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="372" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="373" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="374" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="375" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="376" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="377" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="378" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="379" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="380" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="381" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="382" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="383" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="384" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="385" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="386" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="387" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="388" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="389" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="390" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="391" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="392" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="393" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="394" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="395" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="396" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="397" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="398" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="399" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="400" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="401" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="402" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="403" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="404" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="405" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="406" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="407" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="408" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="409" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="410" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="411" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="412" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="413" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="414" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="415" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="416" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="417" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="418" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="419" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="420" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="421" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="422" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="423" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="424" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="425" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="426" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="427" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="428" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="429" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="430" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="431" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="432" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="433" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="434" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="435" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="436" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="437" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="438" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="439" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="440" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="441" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="442" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="443" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="444" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="445" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="446" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="447" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="448" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="449" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="450" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="451" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="452" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="453" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="454" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="455" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="456" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="457" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="458" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="459" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="460" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="461" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="462" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="463" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="464" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="465" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="466" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="467" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="468" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="469" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="470" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="471" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="472" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="473" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="474" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="475" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="476" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="477" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="478" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="479" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="480" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="481" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="482" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="483" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="484" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="485" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="486" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="487" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="488" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="489" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="490" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="491" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="492" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="493" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="494" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="495" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="496" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="497" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="498" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="499" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="500" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="501" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="502" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="503" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="504" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="505" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="506" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="507" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="508" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="509" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="510" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="511" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="512" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="513" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="514" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="515" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="516" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="517" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="518" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="519" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="520" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="521" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="522" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="523" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="524" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="525" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="526" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="527" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="528" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="529" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="530" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="531" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="532" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="533" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="534" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="535" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="536" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="537" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="538" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="539" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="540" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="541" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="542" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="543" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="544" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="545" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="546" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="547" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="548" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="549" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="550" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="551" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="552" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="553" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="554" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="555" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="556" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="557" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="558" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="559" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="560" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="561" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="562" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="563" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="564" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="565" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="566" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="567" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="568" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="569" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="570" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="571" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="572" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="573" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="574" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="575" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="576" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="577" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="578" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="579" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="580" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="581" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="582" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="583" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="584" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="585" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="586" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="587" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="588" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="589" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="590" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="591" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="592" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="593" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="594" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="595" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="596" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="597" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="598" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="599" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="600" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="601" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="602" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="603" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="604" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="605" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="606" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="607" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="608" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="609" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="610" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="611" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="612" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="613" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="614" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="615" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="616" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="617" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="618" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="619" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="620" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="621" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="622" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="623" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="624" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="625" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="626" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="627" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="628" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="629" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="630" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="631" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="632" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="633" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="634" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="635" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="636" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="637" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="638" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="639" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="640" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="641" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="642" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="643" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="644" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="645" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="646" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="647" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="648" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="649" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="650" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="651" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="652" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="653" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="654" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="655" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="656" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="657" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="658" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="659" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="660" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="661" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="662" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="663" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="664" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="665" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="666" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="667" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="668" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="669" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="670" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="671" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="672" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="673" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="674" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="675" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="676" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="677" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="678" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="679" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="680" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="681" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="682" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="683" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="684" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="685" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="686" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="687" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="688" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="689" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="690" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="691" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="692" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="693" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="694" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="695" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="696" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="697" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="698" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="699" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="700" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="701" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="702" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="703" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="704" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="705" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="706" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="707" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="708" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="709" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="710" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="711" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="712" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="713" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="714" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="715" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="716" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="717" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="718" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="719" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="720" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="721" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="722" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="723" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="724" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="725" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="726" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="727" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="728" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="729" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="730" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="731" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="732" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="733" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="734" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="735" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="736" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="737" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="738" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="739" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="740" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="741" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="742" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="743" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="744" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="745" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="746" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="747" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="748" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="749" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="750" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="751" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="752" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="753" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="754" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="755" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="756" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="757" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="758" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="759" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="760" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="761" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="762" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="763" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="764" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="765" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="766" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="767" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="768" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="769" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="770" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="771" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="772" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="773" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="774" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="775" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="776" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="777" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="778" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="779" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="780" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="781" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="782" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="783" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="784" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="785" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="786" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="787" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="788" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="789" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="790" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="791" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="792" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="793" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="794" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="795" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="796" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="797" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="798" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="799" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="800" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="801" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="802" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="803" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="804" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="805" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="806" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="807" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="808" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="809" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="810" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="811" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="812" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="813" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="814" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="815" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="816" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="817" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="818" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="819" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="820" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="821" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="822" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="823" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="824" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="825" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="826" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="827" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="828" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="829" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="830" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="831" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="832" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="833" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="834" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="835" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="836" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="837" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="838" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="839" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="840" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="841" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="842" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="843" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="844" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="845" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="846" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="847" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="848" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="849" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="850" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="851" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="852" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="853" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="854" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="855" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="856" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="857" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="858" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="859" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="860" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="861" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="862" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="863" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="864" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="865" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="866" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="867" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="868" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="869" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="870" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="871" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="872" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="873" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="874" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="875" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="876" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="877" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="878" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="879" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="880" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="881" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="882" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="883" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="884" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="885" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="886" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="887" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="888" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="889" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="890" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="891" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="892" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="893" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="894" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="895" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="896" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="897" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="898" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="899" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="900" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="901" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="902" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="903" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="904" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="905" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="906" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="907" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="908" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="909" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="910" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="911" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="912" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="913" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="914" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="915" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="916" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="917" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="918" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="919" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="920" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="921" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="922" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="923" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="924" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="925" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="926" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="927" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="928" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="929" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="930" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="931" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="932" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="933" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="934" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="935" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="936" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="937" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="938" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="939" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="940" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="941" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="942" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="943" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="944" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="945" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="946" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="947" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="948" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="949" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="950" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="951" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="952" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="953" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="954" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="955" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="956" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="957" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="958" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="959" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="960" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="961" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="962" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="963" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="964" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="965" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="966" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="967" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="968" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="969" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="970" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="971" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="972" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="973" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="974" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="975" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="976" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="977" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="978" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="979" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="980" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="981" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="982" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="983" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="984" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="985" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="986" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="987" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="988" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="989" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="990" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="991" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="992" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="993" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="994" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="995" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="996" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="997" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="998" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="999" spans="5:25" x14ac:dyDescent="0.25"/>
+    <row r="1000" spans="5:25" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <dataValidations count="26">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="E10:E1000">
+      <formula1>ValidationData!$E$1:$E$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="E2:E1000">
+      <formula1>ValidationData!$E$1:$E$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="F10:F1000">
+      <formula1>ValidationData!$F$1:$F$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="F2:F1000">
+      <formula1>ValidationData!$F$1:$F$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="G10:G1000">
+      <formula1>ValidationData!$G$1:$G$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="G2:G1000">
+      <formula1>ValidationData!$G$1:$G$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="J10:J1000">
+      <formula1>ValidationData!$J$1:$J$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="J2:J1000">
+      <formula1>ValidationData!$J$1:$J$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="M10:M1000">
+      <formula1>ValidationData!$M$1:$M$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="M2:M1000">
+      <formula1>ValidationData!$M$1:$M$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="N10:N1000">
+      <formula1>ValidationData!$N$1:$N$45</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="N2:N1000">
+      <formula1>ValidationData!$N$1:$N$45</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="O10:O1000">
+      <formula1>ValidationData!$O$1:$O$17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="O2:O1000">
+      <formula1>ValidationData!$O$1:$O$17</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="P10:P1000">
+      <formula1>ValidationData!$P$1:$P$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="P2:P1000">
+      <formula1>ValidationData!$P$1:$P$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="Q10:Q1000">
+      <formula1>ValidationData!$Q$1:$Q$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="Q2:Q1000">
+      <formula1>ValidationData!$Q$1:$Q$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="R10:R1000">
+      <formula1>ValidationData!$R$1:$R$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="R2:R1000">
+      <formula1>ValidationData!$R$1:$R$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="S10:S1000">
+      <formula1>ValidationData!$S$1:$S$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="S2:S1000">
+      <formula1>ValidationData!$S$1:$S$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="T10:T1000">
+      <formula1>ValidationData!$T$1:$T$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="information" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." sqref="T2:T1000">
+      <formula1>ValidationData!$T$1:$T$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="Y10:Y1000">
+      <formula1>ValidationData!$Y$1:$Y$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorStyle="stop" errorTitle="Guidance" error="Please select a value from the dropdown list." sqref="Y2:Y1000">
+      <formula1>ValidationData!$Y$1:$Y$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$E$1:$E$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$F$1:$F$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$G$1:$G$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000006000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$J$1:$J$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." xr:uid="{00000000-0002-0000-0000-000008000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$M$1:$M$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>M2:M1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." xr:uid="{00000000-0002-0000-0000-00000A000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$N$1:$N$45</xm:f>
-          </x14:formula1>
-          <xm:sqref>N2:N1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." xr:uid="{00000000-0002-0000-0000-00000C000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$O$1:$O$17</xm:f>
-          </x14:formula1>
-          <xm:sqref>O2:O1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-00000E000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$P$1:$P$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>P2:P1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000010000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$Q$1:$Q$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q2:Q1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000012000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$R$1:$R$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>R2:R1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000014000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$S$1:$S$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>S2:S1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" errorTitle="Invalid Value" error="You can enter multiple values separated by commas. The list is a guide for available options." xr:uid="{00000000-0002-0000-0000-000016000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$T$1:$T$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>T2:T1000</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Value" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000018000000}">
-          <x14:formula1>
-            <xm:f>ValidationData!$Y$1:$Y$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>Y2:Y1000</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:Y45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>25</v>
       </c>
@@ -1170,7 +2232,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>38</v>
       </c>
@@ -1211,7 +2273,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="5:25" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>51</v>
       </c>
@@ -1252,7 +2314,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>64</v>
       </c>
@@ -1281,7 +2343,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
         <v>73</v>
       </c>
@@ -1310,7 +2372,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M6" t="s">
         <v>82</v>
       </c>
@@ -1327,7 +2389,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M7" t="s">
         <v>86</v>
       </c>
@@ -1338,7 +2400,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N8" t="s">
         <v>89</v>
       </c>
@@ -1346,7 +2408,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N9" t="s">
         <v>91</v>
       </c>
@@ -1354,7 +2416,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N10" t="s">
         <v>93</v>
       </c>
@@ -1362,7 +2424,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N11" t="s">
         <v>95</v>
       </c>
@@ -1370,7 +2432,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N12" t="s">
         <v>97</v>
       </c>
@@ -1378,7 +2440,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N13" t="s">
         <v>99</v>
       </c>
@@ -1386,7 +2448,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N14" t="s">
         <v>101</v>
       </c>
@@ -1394,7 +2456,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N15" t="s">
         <v>103</v>
       </c>
@@ -1402,7 +2464,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="5:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N16" t="s">
         <v>105</v>
       </c>
@@ -1410,7 +2472,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N17" t="s">
         <v>107</v>
       </c>
@@ -1418,148 +2480,148 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N19" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N21" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N22" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N23" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N27" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N28" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N29" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N30" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N31" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="14:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N32" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N33" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N34" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N35" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N36" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N37" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N38" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N39" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N40" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N41" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N42" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N43" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N44" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N45" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add validation for email and website fields in SuggestionModal, improve user feedback with toast notifications, and enhance UI consistency in various components including HeroSection and NavUser.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/production/accelerators.xlsx
+++ b/src/lib/scripts/seed-data/production/accelerators.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7125772-D23A-9B4D-A28C-7F7069AF9175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538E5C7D-CC36-1041-A627-8F175466FF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,15 +43,51 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Possible values:
-- in-person
-- remote
-- hybrid</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Possible values:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- in-person
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- remote
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>- hybrid</t>
         </r>
       </text>
     </comment>
@@ -133,17 +169,71 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Possible values:
-- 1-10
-- 11-20
-- 21-50
-- 51-100
-- 100+</t>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Possible values:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- 1-10
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- 11-20
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- 21-50
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">- 51-100
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>- 100+</t>
         </r>
       </text>
     </comment>
@@ -501,7 +591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="164">
   <si>
     <t>name</t>
   </si>
@@ -972,6 +1062,27 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Betaworks</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Company Ventures</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSczMJSQBHRljGqBmv_86qvNzqSBTn5luF2SBEXIQac807cSwg/viewform</t>
+  </si>
+  <si>
+    <t>https://www.companyventures.com/</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>US ONLY</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1116,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1015,6 +1126,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,7 +1163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1060,8 +1177,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1402,27 +1528,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:KU2"/>
+  <dimension ref="A1:KU4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.5" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" style="3" bestFit="1" customWidth="1"/>
@@ -1430,9 +1556,9 @@
     <col min="18" max="18" width="20.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="20" style="3" bestFit="1" customWidth="1"/>
@@ -1809,10 +1935,10 @@
       <c r="KU1" s="2"/>
     </row>
     <row r="2" spans="1:307" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1883,6 +2009,370 @@
       </c>
       <c r="AC2" s="3" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:307" s="5" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
+      <c r="AV3" s="4"/>
+      <c r="AW3" s="4"/>
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4"/>
+      <c r="AZ3" s="4"/>
+      <c r="BA3" s="4"/>
+      <c r="BB3" s="4"/>
+      <c r="BC3" s="4"/>
+      <c r="BD3" s="4"/>
+      <c r="BE3" s="4"/>
+      <c r="BF3" s="4"/>
+      <c r="BG3" s="4"/>
+      <c r="BH3" s="4"/>
+      <c r="BI3" s="4"/>
+      <c r="BJ3" s="4"/>
+      <c r="BK3" s="4"/>
+      <c r="BL3" s="4"/>
+      <c r="BM3" s="4"/>
+      <c r="BN3" s="4"/>
+      <c r="BO3" s="4"/>
+      <c r="BP3" s="4"/>
+      <c r="BQ3" s="4"/>
+      <c r="BR3" s="4"/>
+      <c r="BS3" s="4"/>
+      <c r="BT3" s="4"/>
+      <c r="BU3" s="4"/>
+      <c r="BV3" s="4"/>
+      <c r="BW3" s="4"/>
+      <c r="BX3" s="4"/>
+      <c r="BY3" s="4"/>
+      <c r="BZ3" s="4"/>
+      <c r="CA3" s="4"/>
+      <c r="CB3" s="4"/>
+      <c r="CC3" s="4"/>
+      <c r="CD3" s="4"/>
+      <c r="CE3" s="4"/>
+      <c r="CF3" s="4"/>
+      <c r="CG3" s="4"/>
+      <c r="CH3" s="4"/>
+      <c r="CI3" s="4"/>
+      <c r="CJ3" s="4"/>
+      <c r="CK3" s="4"/>
+      <c r="CL3" s="4"/>
+      <c r="CM3" s="4"/>
+      <c r="CN3" s="4"/>
+      <c r="CO3" s="4"/>
+      <c r="CP3" s="4"/>
+      <c r="CQ3" s="4"/>
+      <c r="CR3" s="4"/>
+      <c r="CS3" s="4"/>
+      <c r="CT3" s="4"/>
+      <c r="CU3" s="4"/>
+      <c r="CV3" s="4"/>
+      <c r="CW3" s="4"/>
+      <c r="CX3" s="4"/>
+      <c r="CY3" s="4"/>
+      <c r="CZ3" s="4"/>
+      <c r="DA3" s="4"/>
+      <c r="DB3" s="4"/>
+      <c r="DC3" s="4"/>
+      <c r="DD3" s="4"/>
+      <c r="DE3" s="4"/>
+      <c r="DF3" s="4"/>
+      <c r="DG3" s="4"/>
+      <c r="DH3" s="4"/>
+      <c r="DI3" s="4"/>
+      <c r="DJ3" s="4"/>
+      <c r="DK3" s="4"/>
+      <c r="DL3" s="4"/>
+      <c r="DM3" s="4"/>
+      <c r="DN3" s="4"/>
+      <c r="DO3" s="4"/>
+      <c r="DP3" s="4"/>
+      <c r="DQ3" s="4"/>
+      <c r="DR3" s="4"/>
+      <c r="DS3" s="4"/>
+      <c r="DT3" s="4"/>
+      <c r="DU3" s="4"/>
+      <c r="DV3" s="4"/>
+      <c r="DW3" s="4"/>
+      <c r="DX3" s="4"/>
+      <c r="DY3" s="4"/>
+      <c r="DZ3" s="4"/>
+      <c r="EA3" s="4"/>
+      <c r="EB3" s="4"/>
+      <c r="EC3" s="4"/>
+      <c r="ED3" s="4"/>
+      <c r="EE3" s="4"/>
+      <c r="EF3" s="4"/>
+      <c r="EG3" s="4"/>
+      <c r="EH3" s="4"/>
+      <c r="EI3" s="4"/>
+      <c r="EJ3" s="4"/>
+      <c r="EK3" s="4"/>
+      <c r="EL3" s="4"/>
+      <c r="EM3" s="4"/>
+      <c r="EN3" s="4"/>
+      <c r="EO3" s="4"/>
+      <c r="EP3" s="4"/>
+      <c r="EQ3" s="4"/>
+      <c r="ER3" s="4"/>
+      <c r="ES3" s="4"/>
+      <c r="ET3" s="4"/>
+      <c r="EU3" s="4"/>
+      <c r="EV3" s="4"/>
+      <c r="EW3" s="4"/>
+      <c r="EX3" s="4"/>
+      <c r="EY3" s="4"/>
+      <c r="EZ3" s="4"/>
+      <c r="FA3" s="4"/>
+      <c r="FB3" s="4"/>
+      <c r="FC3" s="4"/>
+      <c r="FD3" s="4"/>
+      <c r="FE3" s="4"/>
+      <c r="FF3" s="4"/>
+      <c r="FG3" s="4"/>
+      <c r="FH3" s="4"/>
+      <c r="FI3" s="4"/>
+      <c r="FJ3" s="4"/>
+      <c r="FK3" s="4"/>
+      <c r="FL3" s="4"/>
+      <c r="FM3" s="4"/>
+      <c r="FN3" s="4"/>
+      <c r="FO3" s="4"/>
+      <c r="FP3" s="4"/>
+      <c r="FQ3" s="4"/>
+      <c r="FR3" s="4"/>
+      <c r="FS3" s="4"/>
+      <c r="FT3" s="4"/>
+      <c r="FU3" s="4"/>
+      <c r="FV3" s="4"/>
+      <c r="FW3" s="4"/>
+      <c r="FX3" s="4"/>
+      <c r="FY3" s="4"/>
+      <c r="FZ3" s="4"/>
+      <c r="GA3" s="4"/>
+      <c r="GB3" s="4"/>
+      <c r="GC3" s="4"/>
+      <c r="GD3" s="4"/>
+      <c r="GE3" s="4"/>
+      <c r="GF3" s="4"/>
+      <c r="GG3" s="4"/>
+      <c r="GH3" s="4"/>
+      <c r="GI3" s="4"/>
+      <c r="GJ3" s="4"/>
+      <c r="GK3" s="4"/>
+      <c r="GL3" s="4"/>
+      <c r="GM3" s="4"/>
+      <c r="GN3" s="4"/>
+      <c r="GO3" s="4"/>
+      <c r="GP3" s="4"/>
+      <c r="GQ3" s="4"/>
+      <c r="GR3" s="4"/>
+      <c r="GS3" s="4"/>
+      <c r="GT3" s="4"/>
+      <c r="GU3" s="4"/>
+      <c r="GV3" s="4"/>
+      <c r="GW3" s="4"/>
+      <c r="GX3" s="4"/>
+      <c r="GY3" s="4"/>
+      <c r="GZ3" s="4"/>
+      <c r="HA3" s="4"/>
+      <c r="HB3" s="4"/>
+      <c r="HC3" s="4"/>
+      <c r="HD3" s="4"/>
+      <c r="HE3" s="4"/>
+      <c r="HF3" s="4"/>
+      <c r="HG3" s="4"/>
+      <c r="HH3" s="4"/>
+      <c r="HI3" s="4"/>
+      <c r="HJ3" s="4"/>
+      <c r="HK3" s="4"/>
+      <c r="HL3" s="4"/>
+      <c r="HM3" s="4"/>
+      <c r="HN3" s="4"/>
+      <c r="HO3" s="4"/>
+      <c r="HP3" s="4"/>
+      <c r="HQ3" s="4"/>
+      <c r="HR3" s="4"/>
+      <c r="HS3" s="4"/>
+      <c r="HT3" s="4"/>
+      <c r="HU3" s="4"/>
+      <c r="HV3" s="4"/>
+      <c r="HW3" s="4"/>
+      <c r="HX3" s="4"/>
+      <c r="HY3" s="4"/>
+      <c r="HZ3" s="4"/>
+      <c r="IA3" s="4"/>
+      <c r="IB3" s="4"/>
+      <c r="IC3" s="4"/>
+      <c r="ID3" s="4"/>
+      <c r="IE3" s="4"/>
+      <c r="IF3" s="4"/>
+      <c r="IG3" s="4"/>
+      <c r="IH3" s="4"/>
+      <c r="II3" s="4"/>
+      <c r="IJ3" s="4"/>
+      <c r="IK3" s="4"/>
+      <c r="IL3" s="4"/>
+      <c r="IM3" s="4"/>
+      <c r="IN3" s="4"/>
+      <c r="IO3" s="4"/>
+      <c r="IP3" s="4"/>
+      <c r="IQ3" s="4"/>
+      <c r="IR3" s="4"/>
+      <c r="IS3" s="4"/>
+      <c r="IT3" s="4"/>
+      <c r="IU3" s="4"/>
+      <c r="IV3" s="4"/>
+      <c r="IW3" s="4"/>
+      <c r="IX3" s="4"/>
+      <c r="IY3" s="4"/>
+      <c r="IZ3" s="4"/>
+      <c r="JA3" s="4"/>
+      <c r="JB3" s="4"/>
+      <c r="JC3" s="4"/>
+      <c r="JD3" s="4"/>
+      <c r="JE3" s="4"/>
+      <c r="JF3" s="4"/>
+      <c r="JG3" s="4"/>
+      <c r="JH3" s="4"/>
+      <c r="JI3" s="4"/>
+      <c r="JJ3" s="4"/>
+      <c r="JK3" s="4"/>
+      <c r="JL3" s="4"/>
+      <c r="JM3" s="4"/>
+      <c r="JN3" s="4"/>
+      <c r="JO3" s="4"/>
+      <c r="JP3" s="4"/>
+      <c r="JQ3" s="4"/>
+      <c r="JR3" s="4"/>
+      <c r="JS3" s="4"/>
+      <c r="JT3" s="4"/>
+      <c r="JU3" s="4"/>
+      <c r="JV3" s="4"/>
+      <c r="JW3" s="4"/>
+      <c r="JX3" s="4"/>
+      <c r="JY3" s="4"/>
+      <c r="JZ3" s="4"/>
+      <c r="KA3" s="4"/>
+      <c r="KB3" s="4"/>
+      <c r="KC3" s="4"/>
+      <c r="KD3" s="4"/>
+      <c r="KE3" s="4"/>
+      <c r="KF3" s="4"/>
+      <c r="KG3" s="4"/>
+      <c r="KH3" s="4"/>
+      <c r="KI3" s="4"/>
+      <c r="KJ3" s="4"/>
+      <c r="KK3" s="4"/>
+      <c r="KL3" s="4"/>
+      <c r="KM3" s="4"/>
+      <c r="KN3" s="4"/>
+      <c r="KO3" s="4"/>
+      <c r="KP3" s="4"/>
+      <c r="KQ3" s="4"/>
+      <c r="KR3" s="4"/>
+      <c r="KS3" s="4"/>
+      <c r="KT3" s="4"/>
+      <c r="KU3" s="4"/>
+    </row>
+    <row r="4" spans="1:307" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" s="6">
+        <v>44136</v>
+      </c>
+      <c r="K4" s="3">
+        <v>2</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1896,91 +2386,91 @@
           <x14:formula1>
             <xm:f>ValidationData!$AA$1:$AA$3</xm:f>
           </x14:formula1>
-          <xm:sqref>AA2:AA1000</xm:sqref>
+          <xm:sqref>AA2 AA4:AA1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>ValidationData!$E$1:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1000</xm:sqref>
+          <xm:sqref>E2 E5:E1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>ValidationData!$F$1:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1000</xm:sqref>
+          <xm:sqref>F2 F5:F1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>ValidationData!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1000</xm:sqref>
+          <xm:sqref>G2 G5:G1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>ValidationData!$J$1:$J$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1000</xm:sqref>
+          <xm:sqref>J2 J5:J1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
             <xm:f>ValidationData!$M$1:$M$7</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M1000</xm:sqref>
+          <xm:sqref>M2 M4:M1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-00000C000000}">
           <x14:formula1>
             <xm:f>ValidationData!$N$1:$N$45</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N1000</xm:sqref>
+          <xm:sqref>N2 N4:N1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-00000E000000}">
           <x14:formula1>
             <xm:f>ValidationData!$O$1:$O$17</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O1000</xm:sqref>
+          <xm:sqref>O2 O5:O1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000010000000}">
           <x14:formula1>
             <xm:f>ValidationData!$P$1:$P$6</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1000</xm:sqref>
+          <xm:sqref>P2 P5:P1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000012000000}">
           <x14:formula1>
             <xm:f>ValidationData!$Q$1:$Q$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q1000</xm:sqref>
+          <xm:sqref>Q2 Q4:Q1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000014000000}">
           <x14:formula1>
             <xm:f>ValidationData!$R$1:$R$5</xm:f>
           </x14:formula1>
-          <xm:sqref>R2:R1000</xm:sqref>
+          <xm:sqref>R2 R4:R1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000016000000}">
           <x14:formula1>
             <xm:f>ValidationData!$S$1:$S$3</xm:f>
           </x14:formula1>
-          <xm:sqref>S2:S1000</xm:sqref>
+          <xm:sqref>S2 S4:S1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-000018000000}">
           <x14:formula1>
             <xm:f>ValidationData!$T$1:$T$5</xm:f>
           </x14:formula1>
-          <xm:sqref>T2:T1000</xm:sqref>
+          <xm:sqref>T2 T4:T1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-00001A000000}">
           <x14:formula1>
             <xm:f>ValidationData!$Y$1:$Y$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Y2:Y1000</xm:sqref>
+          <xm:sqref>Y2 Y4:Y1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-00001C000000}">
           <x14:formula1>
             <xm:f>ValidationData!$Z$1:$Z$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Z2:Z1000</xm:sqref>
+          <xm:sqref>Z2 Z4:Z1000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
feat: Refactor db-utils and sheet-utils for improved readability; enhance enum handling and update industry types in database schema for better alignment with current definitions.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/production/accelerators.xlsx
+++ b/src/lib/scripts/seed-data/production/accelerators.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26018627-C9CB-414F-8D14-B69E6F6547B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0F79E9-3FA4-A048-8AC6-EF0FFFE090D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="207">
   <si>
     <t>name</t>
   </si>
@@ -894,18 +894,9 @@
     <t>https://airtable.com/apprAAsE4JhFBd8nL/pagGsh6fhh1fzZv6t/form</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Fall 2025</t>
-  </si>
-  <si>
     <t>Pre-seed, Seed</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Focused on product-oriented software startups; flexible capital; mentoring; in-person in SF; community support.</t>
   </si>
   <si>
@@ -918,9 +909,6 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSczMJSQBHRljGqBmv_86qvNzqSBTn5luF2SBEXIQac807cSwg/viewform</t>
   </si>
   <si>
-    <t>Winter 2025</t>
-  </si>
-  <si>
     <t>Sector agnostic but favors FinTech, Health, SaaS; VC check sizes approx. $500K - $1M; strong local NY presence.</t>
   </si>
   <si>
@@ -936,18 +924,12 @@
     <t>Africa, India</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Focus on visionary startups, minority/female founders often; investment includes $50K cash + $150K in-kind; weekly coaching and growth focus.</t>
   </si>
   <si>
     <t>Deep Science Ventures</t>
   </si>
   <si>
-    <t>http://deepscienceventures.com/</t>
-  </si>
-  <si>
     <t>https://www.deepscienceventures.com/contact</t>
   </si>
   <si>
@@ -1015,12 +997,18 @@
   </si>
   <si>
     <t>Pax Momentum offers a profit-driven approach to launching innovative technology companies.</t>
+  </si>
+  <si>
+    <t>https://deepscienceventures.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1077,7 +1065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1087,6 +1075,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1429,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA10" sqref="V3:AA10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1544,8 +1535,8 @@
       <c r="H2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>171</v>
+      <c r="I2" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>30</v>
@@ -1553,11 +1544,11 @@
       <c r="K2" s="1">
         <v>4</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>172</v>
+      <c r="L2" s="4">
+        <v>45672</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>167</v>
@@ -1583,12 +1574,12 @@
       <c r="U2" s="1">
         <v>0</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>174</v>
+      <c r="V2" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>54</v>
@@ -1602,13 +1593,13 @@
     </row>
     <row r="3" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
@@ -1623,8 +1614,8 @@
       <c r="H3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>171</v>
+      <c r="I3" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>45</v>
@@ -1632,11 +1623,11 @@
       <c r="K3" s="1">
         <v>2</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>179</v>
+      <c r="L3" s="4">
+        <v>46327</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>167</v>
@@ -1644,8 +1635,8 @@
       <c r="O3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="P3" s="1">
-        <v>0</v>
+      <c r="P3" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>50</v>
@@ -1662,12 +1653,12 @@
       <c r="U3" s="1">
         <v>0</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>174</v>
+      <c r="V3" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>81</v>
@@ -1681,13 +1672,13 @@
     </row>
     <row r="4" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
@@ -1700,10 +1691,10 @@
         <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
+      </c>
+      <c r="I4" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>45</v>
@@ -1711,17 +1702,17 @@
       <c r="K4" s="1">
         <v>2</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>172</v>
+      <c r="L4" s="4">
+        <v>45672</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>167</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>64</v>
@@ -1741,12 +1732,12 @@
       <c r="U4" s="1">
         <v>0</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>174</v>
+      <c r="V4" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>92</v>
@@ -1760,13 +1751,13 @@
     </row>
     <row r="5" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -1781,8 +1772,8 @@
       <c r="H5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>185</v>
+      <c r="I5" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>45</v>
@@ -1790,11 +1781,11 @@
       <c r="K5" s="1">
         <v>2</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>172</v>
+      <c r="L5" s="4">
+        <v>45672</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>167</v>
@@ -1820,12 +1811,12 @@
       <c r="U5" s="1">
         <v>0</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>174</v>
+      <c r="V5" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>92</v>
@@ -1839,13 +1830,13 @@
     </row>
     <row r="6" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -1860,8 +1851,8 @@
       <c r="H6" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>185</v>
+      <c r="I6" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>45</v>
@@ -1869,11 +1860,11 @@
       <c r="K6" s="1">
         <v>2</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>172</v>
+      <c r="L6" s="4">
+        <v>45672</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>167</v>
@@ -1899,12 +1890,12 @@
       <c r="U6" s="1">
         <v>0</v>
       </c>
-      <c r="V6" s="1" t="s">
-        <v>174</v>
+      <c r="V6" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="Y6" s="1" t="s">
         <v>92</v>
@@ -1918,13 +1909,13 @@
     </row>
     <row r="7" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
@@ -1939,8 +1930,8 @@
       <c r="H7" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>185</v>
+      <c r="I7" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>45</v>
@@ -1948,11 +1939,11 @@
       <c r="K7" s="1">
         <v>2</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>172</v>
+      <c r="L7" s="4">
+        <v>45672</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>167</v>
@@ -1978,12 +1969,12 @@
       <c r="U7" s="1">
         <v>0</v>
       </c>
-      <c r="V7" s="1" t="s">
-        <v>174</v>
+      <c r="V7" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="W7" s="1"/>
       <c r="X7" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>69</v>
@@ -1997,13 +1988,13 @@
     </row>
     <row r="8" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -2018,8 +2009,8 @@
       <c r="H8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>185</v>
+      <c r="I8" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>45</v>
@@ -2027,17 +2018,17 @@
       <c r="K8" s="1">
         <v>2</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>172</v>
+      <c r="L8" s="4">
+        <v>45672</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>84</v>
@@ -2057,12 +2048,12 @@
       <c r="U8" s="1">
         <v>0</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>174</v>
+      <c r="V8" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="W8" s="1"/>
       <c r="X8" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>92</v>
@@ -2076,13 +2067,13 @@
     </row>
     <row r="9" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
@@ -2097,8 +2088,8 @@
       <c r="H9" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>185</v>
+      <c r="I9" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>45</v>
@@ -2106,11 +2097,11 @@
       <c r="K9" s="1">
         <v>2</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>172</v>
+      <c r="L9" s="4">
+        <v>45672</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>167</v>
@@ -2136,12 +2127,12 @@
       <c r="U9" s="1">
         <v>0</v>
       </c>
-      <c r="V9" s="1" t="s">
-        <v>174</v>
+      <c r="V9" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="W9" s="1"/>
       <c r="X9" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="Y9" s="1" t="s">
         <v>92</v>
@@ -2155,13 +2146,13 @@
     </row>
     <row r="10" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
@@ -2176,8 +2167,8 @@
       <c r="H10" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>185</v>
+      <c r="I10" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>45</v>
@@ -2185,11 +2176,11 @@
       <c r="K10" s="1">
         <v>2</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>172</v>
+      <c r="L10" s="4">
+        <v>45672</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>167</v>
@@ -2215,12 +2206,12 @@
       <c r="U10" s="1">
         <v>0</v>
       </c>
-      <c r="V10" s="1" t="s">
-        <v>174</v>
+      <c r="V10" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="W10" s="1"/>
       <c r="X10" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>54</v>
@@ -2234,17 +2225,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{5E763DCA-7788-004D-BC35-316138B91993}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{494BCE2C-0299-8F40-90EB-B7FBD142DCE7}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{81E387C8-EDD2-F440-8312-02B0B2948F35}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{740D4B0D-D2BA-6C48-A72B-5DB296C5D2ED}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{8AE16D84-4859-D348-8C7C-A0DD3A73FC28}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{F0969BB9-7C55-1C42-8AE3-B2F48EA15869}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{74A67E89-2F1B-294B-A1F8-FACB15DE3E43}"/>
-    <hyperlink ref="C6" r:id="rId8" xr:uid="{14BBEFFF-C326-B64A-B617-8B9EFD93BCBF}"/>
-    <hyperlink ref="C7" r:id="rId9" location="_ga=2.203042194.2001170317.1685955250-1964891393.1678098215" display="https://form.typeform.com/to/WlDiIsRh?_gl=1*1e1wi6t*_ga*MTk2NDg5MTM5My4xNjc4MDk4MjE1*_ga_745T7PVTHC*MTcxMzAzMjYxOC42MjcuMS4xNzEzMDMzMTEyLjAuMC4w&amp;typeform-source=foundersfactorystartups.typeform.com#_ga=2.203042194.2001170317.1685955250-1964891393.1678098215" xr:uid="{5AFEC565-224E-FB4B-9FDF-26BB6915A367}"/>
-    <hyperlink ref="C8" r:id="rId10" xr:uid="{7A6E69F7-C0F5-1E41-8453-CCDCE5EC18FB}"/>
-    <hyperlink ref="C9" r:id="rId11" xr:uid="{15BF1A86-50EA-7F40-8174-6C3B02886BD7}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{75546A01-7BCC-BA48-B79D-F8CE2CE6D818}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{D73AC106-470E-EA48-AD7D-FBE18A49E52F}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{D81E1EC6-19D8-DF46-8137-869410B745E1}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{A289598B-29F6-344F-A457-7745E6EAA535}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{BE66E4D8-21FC-B044-838F-ED48BE54E2C1}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{5B0AE72F-7CE3-FC46-9165-E7ACCAAFAE12}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{06A10971-EF0D-A641-B9E5-B876E4E15B71}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{377DB8E9-8DBD-C348-B934-9398FA46C72B}"/>
+    <hyperlink ref="C7" r:id="rId9" location="_ga=2.203042194.2001170317.1685955250-1964891393.1678098215" display="https://form.typeform.com/to/WlDiIsRh?_gl=1*1e1wi6t*_ga*MTk2NDg5MTM5My4xNjc4MDk4MjE1*_ga_745T7PVTHC*MTcxMzAzMjYxOC42MjcuMS4xNzEzMDMzMTEyLjAuMC4w&amp;typeform-source=foundersfactorystartups.typeform.com#_ga=2.203042194.2001170317.1685955250-1964891393.1678098215" xr:uid="{33E6D697-8977-F943-A93E-9F887BB2A356}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{A0638B3B-722C-D140-B573-45415F937AC2}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{397C72A6-B894-3547-809E-FC9A7BCF2AFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
@@ -2256,91 +2247,91 @@
           <x14:formula1>
             <xm:f>ValidationData!$AA$1:$AA$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AA11:AA1000</xm:sqref>
+          <xm:sqref>AA11:AA991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>ValidationData!$E$1:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E11:E1000</xm:sqref>
+          <xm:sqref>E11:E991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>ValidationData!$F$1:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F11:F1000</xm:sqref>
+          <xm:sqref>F11:F991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>ValidationData!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G11:G1000</xm:sqref>
+          <xm:sqref>G11:G991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>ValidationData!$J$1:$J$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J11:J1000</xm:sqref>
+          <xm:sqref>J11:J991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
             <xm:f>ValidationData!$M$1:$M$7</xm:f>
           </x14:formula1>
-          <xm:sqref>M11:M1000</xm:sqref>
+          <xm:sqref>M11:M991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-00000C000000}">
           <x14:formula1>
             <xm:f>ValidationData!$N$1:$N$52</xm:f>
           </x14:formula1>
-          <xm:sqref>N11:N1000</xm:sqref>
+          <xm:sqref>N11:N991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-00000E000000}">
           <x14:formula1>
             <xm:f>ValidationData!$O$1:$O$31</xm:f>
           </x14:formula1>
-          <xm:sqref>O11:O1000</xm:sqref>
+          <xm:sqref>O11:O991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000010000000}">
           <x14:formula1>
             <xm:f>ValidationData!$P$1:$P$6</xm:f>
           </x14:formula1>
-          <xm:sqref>P11:P1000</xm:sqref>
+          <xm:sqref>P11:P991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000012000000}">
           <x14:formula1>
             <xm:f>ValidationData!$Q$1:$Q$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Q11:Q1000</xm:sqref>
+          <xm:sqref>Q11:Q991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000014000000}">
           <x14:formula1>
             <xm:f>ValidationData!$R$1:$R$5</xm:f>
           </x14:formula1>
-          <xm:sqref>R11:R1000</xm:sqref>
+          <xm:sqref>R11:R991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000016000000}">
           <x14:formula1>
             <xm:f>ValidationData!$S$1:$S$3</xm:f>
           </x14:formula1>
-          <xm:sqref>S11:S1000</xm:sqref>
+          <xm:sqref>S11:S991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-000018000000}">
           <x14:formula1>
             <xm:f>ValidationData!$T$1:$T$4</xm:f>
           </x14:formula1>
-          <xm:sqref>T11:T1000</xm:sqref>
+          <xm:sqref>T11:T991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-00001A000000}">
           <x14:formula1>
             <xm:f>ValidationData!$Y$1:$Y$5</xm:f>
           </x14:formula1>
-          <xm:sqref>Y11:Y1000</xm:sqref>
+          <xm:sqref>Y11:Y991</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-00001C000000}">
           <x14:formula1>
             <xm:f>ValidationData!$Z$1:$Z$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Z11:Z1000</xm:sqref>
+          <xm:sqref>Z11:Z991</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
refactor: Standardize audio playback error handling across multiple components and remove references to 'Korea' and 'Oceania' in region checks.
</commit_message>
<xml_diff>
--- a/src/lib/scripts/seed-data/production/accelerators.xlsx
+++ b/src/lib/scripts/seed-data/production/accelerators.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0F79E9-3FA4-A048-8AC6-EF0FFFE090D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40105AEF-0500-4448-B28E-247F8EE0C9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -897,9 +897,6 @@
     <t>Pre-seed, Seed</t>
   </si>
   <si>
-    <t>Focused on product-oriented software startups; flexible capital; mentoring; in-person in SF; community support.</t>
-  </si>
-  <si>
     <t>Company Ventures</t>
   </si>
   <si>
@@ -909,9 +906,6 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSczMJSQBHRljGqBmv_86qvNzqSBTn5luF2SBEXIQac807cSwg/viewform</t>
   </si>
   <si>
-    <t>Sector agnostic but favors FinTech, Health, SaaS; VC check sizes approx. $500K - $1M; strong local NY presence.</t>
-  </si>
-  <si>
     <t>Expert DOJO</t>
   </si>
   <si>
@@ -924,18 +918,12 @@
     <t>Africa, India</t>
   </si>
   <si>
-    <t>Focus on visionary startups, minority/female founders often; investment includes $50K cash + $150K in-kind; weekly coaching and growth focus.</t>
-  </si>
-  <si>
     <t>Deep Science Ventures</t>
   </si>
   <si>
     <t>https://www.deepscienceventures.com/contact</t>
   </si>
   <si>
-    <t>DSV is a venture studio and a fund that develops a systematic, optimized approach to science company development and investment.</t>
-  </si>
-  <si>
     <t>Highline Beta</t>
   </si>
   <si>
@@ -945,9 +933,6 @@
     <t>https://www.highlinebeta.com/contact-us</t>
   </si>
   <si>
-    <t>Highline Beta is a startup co-creation company that launches new ventures with leading corporations and founders.</t>
-  </si>
-  <si>
     <t>Founders Factory</t>
   </si>
   <si>
@@ -984,9 +969,6 @@
     <t>https://katapult.vc/get-in-touch-with-katapult/</t>
   </si>
   <si>
-    <t>Katapult is an investment company and accelerator, focused on highly scalable impact climate, ocean and agri-tech startups.</t>
-  </si>
-  <si>
     <t>Pax Momentum</t>
   </si>
   <si>
@@ -1000,6 +982,24 @@
   </si>
   <si>
     <t>https://deepscienceventures.com/</t>
+  </si>
+  <si>
+    <t>They focus on product-oriented software startups, providing flexible capital, mentoring, in-person support in San Francisco, and community backing.</t>
+  </si>
+  <si>
+    <t>They are sector agnostic but favor FinTech, Health, and SaaS companies, writing VC checks of approximately $500K to $1M with a strong local New York presence.</t>
+  </si>
+  <si>
+    <t>They focus on visionary startups, often supporting minority and female founders, with investments that include $50K cash plus $150K in-kind support, weekly coaching, and growth-focused guidance.</t>
+  </si>
+  <si>
+    <t>DSV is a venture studio and fund that develops a systematic, optimized approach to science company development and investment.</t>
+  </si>
+  <si>
+    <t>Highline Beta is a startup co-creation company that launches new ventures with leading corporations and founders.RetryClaude can make mistakes. Please double-check responses.</t>
+  </si>
+  <si>
+    <t>Katapult is an investment company and accelerator focused on highly scalable impact climate, ocean and agri-tech startups.</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1007,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1076,7 +1076,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>54</v>
@@ -1593,13 +1593,13 @@
     </row>
     <row r="3" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>81</v>
@@ -1672,13 +1672,13 @@
     </row>
     <row r="4" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
@@ -1691,7 +1691,7 @@
         <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I4" s="1" t="b">
         <v>1</v>
@@ -1712,7 +1712,7 @@
         <v>167</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>64</v>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>92</v>
@@ -1751,13 +1751,13 @@
     </row>
     <row r="5" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>92</v>
@@ -1830,13 +1830,13 @@
     </row>
     <row r="6" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -1895,7 +1895,7 @@
       </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="Y6" s="1" t="s">
         <v>92</v>
@@ -1909,13 +1909,13 @@
     </row>
     <row r="7" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="W7" s="1"/>
       <c r="X7" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>69</v>
@@ -1988,13 +1988,13 @@
     </row>
     <row r="8" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -2025,10 +2025,10 @@
         <v>171</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>84</v>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="W8" s="1"/>
       <c r="X8" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>92</v>
@@ -2067,13 +2067,13 @@
     </row>
     <row r="9" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="W9" s="1"/>
       <c r="X9" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="Y9" s="1" t="s">
         <v>92</v>
@@ -2146,13 +2146,13 @@
     </row>
     <row r="10" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
@@ -2211,7 +2211,7 @@
       </c>
       <c r="W10" s="1"/>
       <c r="X10" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>54</v>
@@ -2225,17 +2225,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{75546A01-7BCC-BA48-B79D-F8CE2CE6D818}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{D73AC106-470E-EA48-AD7D-FBE18A49E52F}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{D81E1EC6-19D8-DF46-8137-869410B745E1}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{A289598B-29F6-344F-A457-7745E6EAA535}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{BE66E4D8-21FC-B044-838F-ED48BE54E2C1}"/>
-    <hyperlink ref="B10" r:id="rId6" xr:uid="{5B0AE72F-7CE3-FC46-9165-E7ACCAAFAE12}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{06A10971-EF0D-A641-B9E5-B876E4E15B71}"/>
-    <hyperlink ref="C6" r:id="rId8" xr:uid="{377DB8E9-8DBD-C348-B934-9398FA46C72B}"/>
-    <hyperlink ref="C7" r:id="rId9" location="_ga=2.203042194.2001170317.1685955250-1964891393.1678098215" display="https://form.typeform.com/to/WlDiIsRh?_gl=1*1e1wi6t*_ga*MTk2NDg5MTM5My4xNjc4MDk4MjE1*_ga_745T7PVTHC*MTcxMzAzMjYxOC42MjcuMS4xNzEzMDMzMTEyLjAuMC4w&amp;typeform-source=foundersfactorystartups.typeform.com#_ga=2.203042194.2001170317.1685955250-1964891393.1678098215" xr:uid="{33E6D697-8977-F943-A93E-9F887BB2A356}"/>
-    <hyperlink ref="C8" r:id="rId10" xr:uid="{A0638B3B-722C-D140-B573-45415F937AC2}"/>
-    <hyperlink ref="C9" r:id="rId11" xr:uid="{397C72A6-B894-3547-809E-FC9A7BCF2AFE}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{87F2E127-0BE0-824E-BF3E-404D9B374564}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{CE730559-B643-A140-ACA4-4FFCBC7939D0}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{3649F6D0-E097-2345-A0AC-9BD8FB5B4996}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{813B7D81-417D-F24C-8714-9538455F0C68}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{5BB7C7B8-C6D9-974D-86FD-796390807641}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{4ED6FA8A-9B88-DD45-B2B6-568A255C50EB}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{D1B602DB-2D95-B547-B753-D3F11D76F13B}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{1E4E0B91-6F50-D343-9AB1-6A3783DAD811}"/>
+    <hyperlink ref="C7" r:id="rId9" location="_ga=2.203042194.2001170317.1685955250-1964891393.1678098215" display="https://form.typeform.com/to/WlDiIsRh?_gl=1*1e1wi6t*_ga*MTk2NDg5MTM5My4xNjc4MDk4MjE1*_ga_745T7PVTHC*MTcxMzAzMjYxOC42MjcuMS4xNzEzMDMzMTEyLjAuMC4w&amp;typeform-source=foundersfactorystartups.typeform.com#_ga=2.203042194.2001170317.1685955250-1964891393.1678098215" xr:uid="{93F8BDE3-BA7F-6C47-A4A9-98A04B01D238}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{49472879-5384-FF49-A1B2-721BA27C7691}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{052D5142-CA4C-1942-B162-B10DBC51693C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
@@ -2247,91 +2247,91 @@
           <x14:formula1>
             <xm:f>ValidationData!$AA$1:$AA$4</xm:f>
           </x14:formula1>
-          <xm:sqref>AA11:AA991</xm:sqref>
+          <xm:sqref>AA11:AA982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>ValidationData!$E$1:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E11:E991</xm:sqref>
+          <xm:sqref>E11:E982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>ValidationData!$F$1:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F11:F991</xm:sqref>
+          <xm:sqref>F11:F982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>ValidationData!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G11:G991</xm:sqref>
+          <xm:sqref>G11:G982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>ValidationData!$J$1:$J$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J11:J991</xm:sqref>
+          <xm:sqref>J11:J982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
             <xm:f>ValidationData!$M$1:$M$7</xm:f>
           </x14:formula1>
-          <xm:sqref>M11:M991</xm:sqref>
+          <xm:sqref>M11:M982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-00000C000000}">
           <x14:formula1>
             <xm:f>ValidationData!$N$1:$N$52</xm:f>
           </x14:formula1>
-          <xm:sqref>N11:N991</xm:sqref>
+          <xm:sqref>N11:N982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-00000E000000}">
           <x14:formula1>
             <xm:f>ValidationData!$O$1:$O$31</xm:f>
           </x14:formula1>
-          <xm:sqref>O11:O991</xm:sqref>
+          <xm:sqref>O11:O982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000010000000}">
           <x14:formula1>
             <xm:f>ValidationData!$P$1:$P$6</xm:f>
           </x14:formula1>
-          <xm:sqref>P11:P991</xm:sqref>
+          <xm:sqref>P11:P982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000012000000}">
           <x14:formula1>
             <xm:f>ValidationData!$Q$1:$Q$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Q11:Q991</xm:sqref>
+          <xm:sqref>Q11:Q982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000014000000}">
           <x14:formula1>
             <xm:f>ValidationData!$R$1:$R$5</xm:f>
           </x14:formula1>
-          <xm:sqref>R11:R991</xm:sqref>
+          <xm:sqref>R11:R982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-000016000000}">
           <x14:formula1>
             <xm:f>ValidationData!$S$1:$S$3</xm:f>
           </x14:formula1>
-          <xm:sqref>S11:S991</xm:sqref>
+          <xm:sqref>S11:S982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Select a value from the list, or enter multiple values separated by commas or semicolons." xr:uid="{00000000-0002-0000-0000-000018000000}">
           <x14:formula1>
             <xm:f>ValidationData!$T$1:$T$4</xm:f>
           </x14:formula1>
-          <xm:sqref>T11:T991</xm:sqref>
+          <xm:sqref>T11:T982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-00001A000000}">
           <x14:formula1>
             <xm:f>ValidationData!$Y$1:$Y$5</xm:f>
           </x14:formula1>
-          <xm:sqref>Y11:Y991</xm:sqref>
+          <xm:sqref>Y11:Y982</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Guidance" error="Please select a value from the dropdown list." xr:uid="{00000000-0002-0000-0000-00001C000000}">
           <x14:formula1>
             <xm:f>ValidationData!$Z$1:$Z$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Z11:Z991</xm:sqref>
+          <xm:sqref>Z11:Z982</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>